<commit_message>
Added framework code and practice code
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B07A40-B218-4EBA-87A5-E151350737EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75815339-E794-48E6-A5D7-D220DC207A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,12 +554,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5045475-3480-43C6-AFFA-755CC2BF10EF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
     <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -609,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77AD6F-85AD-4D0C-B227-94C64C76B708}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added delete API to the framework
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75815339-E794-48E6-A5D7-D220DC207A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F836BC6-74FA-4A03-8276-C7776DC2353B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>email</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>DescriptionTestEngineer2(cxCreationInvalidKey)</t>
+  </si>
+  <si>
+    <t>deleteCustomer</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>test4@mailinator.com</t>
+  </si>
+  <si>
+    <t>test5@mailinator.com</t>
+  </si>
+  <si>
+    <t>cus_OdRXAoRWnlPwpG</t>
   </si>
 </sst>
 </file>
@@ -140,9 +155,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -424,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
   </cols>
@@ -533,6 +551,21 @@
       </c>
       <c r="C11" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -554,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5045475-3480-43C6-AFFA-755CC2BF10EF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +614,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -592,7 +625,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added paralle test running and extent reports
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F836BC6-74FA-4A03-8276-C7776DC2353B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C889B9B6-4ABC-4C90-AD7C-A12741924443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <t>test5@mailinator.com</t>
   </si>
   <si>
-    <t>cus_OdRXAoRWnlPwpG</t>
+    <t>cus_OdRXZBEHaTVxA4</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
minor changes in testng.xml
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F46CD9-E758-4CA5-BA67-1E33D217D901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F062279F-9D86-42E1-807C-4C042F114F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <t>test5@mailinator.com</t>
   </si>
   <si>
-    <t>cus_OdV0owPLzqhT7n</t>
+    <t>cus_OdV9ggDYK3xZVr</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added methods to fetch key value using jsonpath
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F062279F-9D86-42E1-807C-4C042F114F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520D3B0-86FE-4258-944B-64628C70D149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <t>test5@mailinator.com</t>
   </si>
   <si>
-    <t>cus_OdV9ggDYK3xZVr</t>
+    <t>cus_OdVhGd9iTYfzfB</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -587,14 +587,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5045475-3480-43C6-AFFA-755CC2BF10EF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Updated test data and validating jenkins is executing test after pushing to github
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520D3B0-86FE-4258-944B-64628C70D149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA25A75B-97B6-4134-8586-EC21D7AB0103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>email</t>
   </si>
@@ -105,6 +105,42 @@
   </si>
   <si>
     <t>cus_OdVhGd9iTYfzfB</t>
+  </si>
+  <si>
+    <t>testEngineer4</t>
+  </si>
+  <si>
+    <t>testEngineer5</t>
+  </si>
+  <si>
+    <t>testEngineer6</t>
+  </si>
+  <si>
+    <t>test6@mailinator.com</t>
+  </si>
+  <si>
+    <t>testEngineer7</t>
+  </si>
+  <si>
+    <t>testEngineer8</t>
+  </si>
+  <si>
+    <t>test7@mailinator.com</t>
+  </si>
+  <si>
+    <t>test8@mailinator.com</t>
+  </si>
+  <si>
+    <t>testEngineer9</t>
+  </si>
+  <si>
+    <t>testEngineer10</t>
+  </si>
+  <si>
+    <t>test9@mailinator.com</t>
+  </si>
+  <si>
+    <t>test10@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -444,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,10 +558,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -533,10 +569,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -544,10 +580,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -587,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5045475-3480-43C6-AFFA-755CC2BF10EF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,10 +647,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -622,10 +658,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -644,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77AD6F-85AD-4D0C-B227-94C64C76B708}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,10 +704,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -679,10 +715,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added paypal 2 request
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/src/test/java/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\src\test\java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA25A75B-97B6-4134-8586-EC21D7AB0103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8E06FA-434B-4FF5-9101-E89A69D1D34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>test5@mailinator.com</t>
   </si>
   <si>
-    <t>cus_OdVhGd9iTYfzfB</t>
-  </si>
-  <si>
     <t>testEngineer4</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>test10@mailinator.com</t>
+  </si>
+  <si>
+    <t>cus_OehjJmR5GBWHrF</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -647,10 +647,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -658,10 +658,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -680,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77AD6F-85AD-4D0C-B227-94C64C76B708}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
@@ -704,10 +704,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -715,10 +715,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>

</xml_diff>